<commit_message>
fix(API): Ajustes na lingua chinesa, inclusão de novas linguagens para analise de dados com descrição correta
</commit_message>
<xml_diff>
--- a/back/API/dados/coletaDeDados.xlsx
+++ b/back/API/dados/coletaDeDados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1915,6 +1915,3491 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>es-ES</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Buen día</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>18-06-2024 10:02:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>es-ES</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Buen día</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>18-06-2024 10:06:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>tr</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Günaydin</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>18-06-2024 10:10:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>18-06-2024 10:35:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:44:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:45:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:46:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:46:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:47:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:47:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:47:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:48:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:48:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:48:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:52:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:53:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:55:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>18-06-2024 11:55:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>sv</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Bom di</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>God morgon</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:06:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>sv</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>God morgon</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:07:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>tr</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Em que posso ajudar?</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Nasıl yardımcı olabilirim?</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:07:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>nl</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Gosto da inglaterra</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Ik hou van engeland</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:07:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Buongiorno</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:08:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>es-ES</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Buen día</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:13:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Buongiorno</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:15:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:16:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:16:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Prüfen</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:20:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>en-usa</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Alo</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:20:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>en-usa</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:20:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>en-usa</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:21:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>es-ES</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Hola</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:22:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" t="b">
+        <v>1</v>
+      </c>
+      <c r="H71" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:23:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>es-ES</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Buen día</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="b">
+        <v>1</v>
+      </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="b">
+        <v>1</v>
+      </c>
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:24:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Quem fala</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Who speaks</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:24:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>es-ES</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Buen día</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="b">
+        <v>1</v>
+      </c>
+      <c r="H75" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:31:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="b">
+        <v>1</v>
+      </c>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:32:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Que dia é hoje?</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>What day is today?</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:32:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>صباح الخير</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:33:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>ko</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>안녕하세요</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>1</v>
+      </c>
+      <c r="H79" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:34:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+      <c r="H80" t="b">
+        <v>0</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:34:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ko</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>안녕하세요</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" t="b">
+        <v>1</v>
+      </c>
+      <c r="H81" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:34:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ko</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>I have a big dick</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>나는 큰 거시기가있다</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F82" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" t="b">
+        <v>1</v>
+      </c>
+      <c r="H82" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:35:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:35:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+      <c r="H84" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:36:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" t="b">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:36:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:36:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>en-us</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Quero cu</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>I want ass</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="b">
+        <v>1</v>
+      </c>
+      <c r="H87" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:36:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>शुभ प्रभात</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" t="b">
+        <v>1</v>
+      </c>
+      <c r="H88" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:37:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>en-usd</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" t="b">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:38:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>en-usd</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:40:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>en-usd</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+      <c r="G91" t="b">
+        <v>1</v>
+      </c>
+      <c r="H91" t="b">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:41:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>tr</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Günaydın</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F92" t="b">
+        <v>0</v>
+      </c>
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+      <c r="H92" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:48:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>sv</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>God morgon</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F93" t="b">
+        <v>0</v>
+      </c>
+      <c r="G93" t="b">
+        <v>1</v>
+      </c>
+      <c r="H93" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:48:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>pl</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Dzień dobry</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F94" t="b">
+        <v>0</v>
+      </c>
+      <c r="G94" t="b">
+        <v>1</v>
+      </c>
+      <c r="H94" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:48:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>en-usd</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:52:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>en-usd</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:54:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>es-ES</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Que dia é hoje</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Qué día es hoy</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F97" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:54:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>शुभ प्रभात</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>18-06-2024 12:55:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>pt-br</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>zh-CN</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>早上好</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F99" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F100" t="b">
+        <v>1</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:07:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:07:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Buen día</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F102" t="b">
+        <v>1</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:07:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Buen dia</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F103" t="b">
+        <v>1</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:08:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>zh-CN</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>早上好</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F104" t="b">
+        <v>1</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:08:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>zh-CN</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Que dia é hoje?</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>今天是什么日子？</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F105" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:08:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>zh-CN</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>早上好</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F106" t="b">
+        <v>1</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:08:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>zh-CN</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>早上好</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F107" t="b">
+        <v>0</v>
+      </c>
+      <c r="G107" t="b">
+        <v>1</v>
+      </c>
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:08:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F108" t="b">
+        <v>0</v>
+      </c>
+      <c r="G108" t="b">
+        <v>1</v>
+      </c>
+      <c r="H108" t="b">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:08:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F109" t="b">
+        <v>0</v>
+      </c>
+      <c r="G109" t="b">
+        <v>1</v>
+      </c>
+      <c r="H109" t="b">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:09:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Que dia é hoje</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>आज कोन सा दिन हे</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F110" t="b">
+        <v>0</v>
+      </c>
+      <c r="G110" t="b">
+        <v>1</v>
+      </c>
+      <c r="H110" t="b">
+        <v>0</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:09:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>शुभ प्रभात</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F111" t="b">
+        <v>0</v>
+      </c>
+      <c r="G111" t="b">
+        <v>1</v>
+      </c>
+      <c r="H111" t="b">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:09:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Доброе утро</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F112" t="b">
+        <v>0</v>
+      </c>
+      <c r="G112" t="b">
+        <v>1</v>
+      </c>
+      <c r="H112" t="b">
+        <v>0</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:09:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>ru</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Que dia é hoje manito</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Какой сегодня день</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F113" t="b">
+        <v>0</v>
+      </c>
+      <c r="G113" t="b">
+        <v>1</v>
+      </c>
+      <c r="H113" t="b">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:10:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>शुभ प्रभात</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F114" t="b">
+        <v>0</v>
+      </c>
+      <c r="G114" t="b">
+        <v>1</v>
+      </c>
+      <c r="H114" t="b">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:11:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>おはよう</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F115" t="b">
+        <v>0</v>
+      </c>
+      <c r="G115" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" t="b">
+        <v>0</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:12:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F116" t="b">
+        <v>0</v>
+      </c>
+      <c r="G116" t="b">
+        <v>1</v>
+      </c>
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:30:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F117" t="b">
+        <v>0</v>
+      </c>
+      <c r="G117" t="b">
+        <v>1</v>
+      </c>
+      <c r="H117" t="b">
+        <v>0</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:30:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>صباح الخير</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F118" t="b">
+        <v>0</v>
+      </c>
+      <c r="G118" t="b">
+        <v>1</v>
+      </c>
+      <c r="H118" t="b">
+        <v>0</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:31:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Que dia é hoje</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>What day is today</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F119" t="b">
+        <v>0</v>
+      </c>
+      <c r="G119" t="b">
+        <v>1</v>
+      </c>
+      <c r="H119" t="b">
+        <v>0</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:31:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>صباح الخير</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F120" t="b">
+        <v>0</v>
+      </c>
+      <c r="G120" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120" t="b">
+        <v>0</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:32:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Não sei oque dizer a mais</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>لا أعرف ما أقوله أكثر</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F121" t="b">
+        <v>0</v>
+      </c>
+      <c r="G121" t="b">
+        <v>1</v>
+      </c>
+      <c r="H121" t="b">
+        <v>0</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>18-06-2024 13:33:13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix(API/Archives): Arquivos e configuração da API ajustados para funcionar na web 24/7
</commit_message>
<xml_diff>
--- a/back/API/dados/coletaDeDados.xlsx
+++ b/back/API/dados/coletaDeDados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Japonês</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,84 +503,84 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>おはよう</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>18-06-2024 21:26:52</t>
+          <t>19-06-2024 20:01:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Francês</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Good morning</t>
+          <t>Alo</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bonjour</t>
+          <t>Hello</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>18-06-2024 21:27:01</t>
+          <t>19-06-2024 20:01:56</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Francês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -590,12 +590,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bonjour</t>
+          <t>Que dia é hoje</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Good morning</t>
+          <t>What day is today</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -619,29 +619,29 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>18-06-2024 21:27:11</t>
+          <t>19-06-2024 20:02:10</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>How are you</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>어떻게 지내세요</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -665,329 +665,329 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>18-06-2024 21:29:15</t>
+          <t>19-06-2024 20:03:49</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>월요일</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>18-06-2024 21:33:39</t>
+          <t>19-06-2024 20:04:24</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Alo</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>토요일</t>
+          <t>Hello</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>18-06-2024 21:33:42</t>
+          <t>19-06-2024 20:05:38</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>금요일</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>18-06-2024 21:33:46</t>
+          <t>19-06-2024 20:09:28</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Chese</t>
+          <t>Caralho</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Chese</t>
+          <t>Fuck</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:03</t>
+          <t>19-06-2024 20:11:53</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Turco</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>월요일</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Pazartesi</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:26</t>
+          <t>19-06-2024 20:12:26</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Turco</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>토요일</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Cumartesi</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:30</t>
+          <t>19-06-2024 20:12:34</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Coreano</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Turco</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>금요일</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Cuma</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:32</t>
+          <t>19-06-2024 20:14:05</t>
         </is>
       </c>
     </row>
@@ -999,41 +999,41 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Russo</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bunda</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Приклад</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:43</t>
+          <t>19-06-2024 20:19:06</t>
         </is>
       </c>
     </row>
@@ -1045,41 +1045,41 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Russo</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Feijão</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Фасоль</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:47</t>
+          <t>19-06-2024 20:19:17</t>
         </is>
       </c>
     </row>
@@ -1091,41 +1091,41 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Russo</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Arroz</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Рис</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:48</t>
+          <t>19-06-2024 20:20:35</t>
         </is>
       </c>
     </row>
@@ -1137,41 +1137,41 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Russo</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Coxa</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Бедро</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>18-06-2024 21:34:57</t>
+          <t>19-06-2024 20:20:54</t>
         </is>
       </c>
     </row>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Russo</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1193,31 +1193,31 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Доброе утро</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>18-06-2024 21:35:05</t>
+          <t>19-06-2024 20:21:01</t>
         </is>
       </c>
     </row>
@@ -1229,41 +1229,41 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Russo</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Minha filha é alta</t>
+          <t>Aaaaaaaaaaaaaa</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Моя дочь высокая</t>
+          <t>Aaaaaaaaaaaaaa</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>18-06-2024 21:35:17</t>
+          <t>19-06-2024 20:21:05</t>
         </is>
       </c>
     </row>
@@ -1275,41 +1275,41 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Russo</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Galinha</t>
+          <t>Faca</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Курица</t>
+          <t>Do</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>18-06-2024 21:35:31</t>
+          <t>19-06-2024 20:29:11</t>
         </is>
       </c>
     </row>
@@ -1321,41 +1321,41 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Chinês</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Feijão</t>
+          <t>Faca</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>豆</t>
+          <t>Do</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Chrome</t>
+          <t>Chrome Mobile</t>
         </is>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Windows</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>18-06-2024 21:35:46</t>
+          <t>19-06-2024 20:29:43</t>
         </is>
       </c>
     </row>
@@ -1367,41 +1367,869 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:31:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Salve</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Save</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:31:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:36:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:36:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Boa tarde</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Good afternoon</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:36:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:39:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Amigo</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Friend</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:39:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:41:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Good morning</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:41:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Amigo</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Friend</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>19-06-2024 20:41:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>Chinês</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Feijão</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>豆</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Chrome</t>
-        </is>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Linux</t>
-        </is>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>18-06-2024 21:36:06</t>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>早上好</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:19:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Chinês</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>早上好</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:20:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Chinês</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Meu pau na sua mao</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>我的公鸡在你的手里</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:20:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Chinês</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Fala direito</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>言语正确</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:20:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Que dia é hoje malandro?</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>今天是哪一天的騙子？</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:21:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:21:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:21:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Que dia é hoje</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>What day is today</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:21:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Fala comigo jão se não eu vou pegar você pelo cangote</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Talk to me jão if not i will take you for the neck</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Chrome Mobile</t>
+        </is>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Android</t>
+        </is>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>21-06-2024 12:22:10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(Readme): Ajuste no arquivo README
</commit_message>
<xml_diff>
--- a/back/API/dados/coletaDeDados.xlsx
+++ b/back/API/dados/coletaDeDados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2233,6 +2233,282 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Bom dia, gostaria de falar com o senhor pedro</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Good morning, i would like to talk to mr. pedro</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:25:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Seria possível?</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>It would be possible?</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:25:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Yes, one momento please!</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Sim, um momento, por favor!</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:25:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Posso me sentar aqui?</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>May i sit here?</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:26:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Yes, feel free</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Sim, sinta -se livre</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:26:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Mr. pedro will talk to you soon, okay?</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>O sr. pedro falará com você em breve, ok?</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:27:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(new-dados): Novos dados adicionados
</commit_message>
<xml_diff>
--- a/back/API/dados/coletaDeDados.xlsx
+++ b/back/API/dados/coletaDeDados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2233,6 +2233,282 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Bom dia, gostaria de falar com o senhor pedro</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Good morning, i would like to talk to mr. pedro</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:25:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Seria possível?</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>It would be possible?</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:25:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Yes, one momento please!</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Sim, um momento, por favor!</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:25:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Posso me sentar aqui?</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>May i sit here?</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:26:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Yes, feel free</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Sim, sinta -se livre</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:26:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Mr. pedro will talk to you soon, okay?</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>O sr. pedro falará com você em breve, ok?</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>23-06-2024 11:27:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(analiseProfunda): Adição do arquivo para analise de dados
</commit_message>
<xml_diff>
--- a/back/API/dados/coletaDeDados.xlsx
+++ b/back/API/dados/coletaDeDados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -820,12 +820,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Caralho</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Fuck</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>19-06-2024 20:11:53</t>
+          <t>19-06-2024 20:12:26</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>19-06-2024 20:12:26</t>
+          <t>19-06-2024 20:12:34</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>19-06-2024 20:12:34</t>
+          <t>19-06-2024 20:14:05</t>
         </is>
       </c>
     </row>
@@ -987,7 +987,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>19-06-2024 20:14:05</t>
+          <t>19-06-2024 20:19:06</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>19-06-2024 20:19:06</t>
+          <t>19-06-2024 20:19:17</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>19-06-2024 20:19:17</t>
+          <t>19-06-2024 20:20:35</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>19-06-2024 20:20:35</t>
+          <t>19-06-2024 20:20:54</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>19-06-2024 20:20:54</t>
+          <t>19-06-2024 20:21:01</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>19-06-2024 20:21:01</t>
+          <t>19-06-2024 20:31:26</t>
         </is>
       </c>
     </row>
@@ -1234,12 +1234,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Aaaaaaaaaaaaaa</t>
+          <t>Salve</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Aaaaaaaaaaaaaa</t>
+          <t>Save</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>19-06-2024 20:21:05</t>
+          <t>19-06-2024 20:31:41</t>
         </is>
       </c>
     </row>
@@ -1280,12 +1280,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Faca</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Do</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>19-06-2024 20:29:11</t>
+          <t>19-06-2024 20:36:31</t>
         </is>
       </c>
     </row>
@@ -1326,12 +1326,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Faca</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Do</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>19-06-2024 20:29:43</t>
+          <t>19-06-2024 20:36:39</t>
         </is>
       </c>
     </row>
@@ -1372,12 +1372,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Boa tarde</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Good morning</t>
+          <t>Good afternoon</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>19-06-2024 20:31:26</t>
+          <t>19-06-2024 20:36:43</t>
         </is>
       </c>
     </row>
@@ -1418,12 +1418,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Salve</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Save</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>19-06-2024 20:31:41</t>
+          <t>19-06-2024 20:39:13</t>
         </is>
       </c>
     </row>
@@ -1464,12 +1464,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Amigo</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Good morning</t>
+          <t>Friend</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>19-06-2024 20:36:31</t>
+          <t>19-06-2024 20:39:18</t>
         </is>
       </c>
     </row>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>19-06-2024 20:36:39</t>
+          <t>19-06-2024 20:41:08</t>
         </is>
       </c>
     </row>
@@ -1556,12 +1556,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Boa tarde</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Good afternoon</t>
+          <t>Good morning</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>19-06-2024 20:36:43</t>
+          <t>19-06-2024 20:41:42</t>
         </is>
       </c>
     </row>
@@ -1602,12 +1602,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Amigo</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Good morning</t>
+          <t>Friend</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>19-06-2024 20:39:13</t>
+          <t>19-06-2024 20:41:45</t>
         </is>
       </c>
     </row>
@@ -1643,17 +1643,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Chinês</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Amigo</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Friend</t>
+          <t>早上好</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>19-06-2024 20:39:18</t>
+          <t>21-06-2024 12:19:40</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Chinês</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Good morning</t>
+          <t>早上好</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>19-06-2024 20:41:08</t>
+          <t>21-06-2024 12:20:34</t>
         </is>
       </c>
     </row>
@@ -1735,17 +1735,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Chinês</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Fala direito</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Good morning</t>
+          <t>言语正确</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1769,29 +1769,29 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>19-06-2024 20:41:42</t>
+          <t>21-06-2024 12:20:59</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Taiwan</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Amigo</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Friend</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1815,19 +1815,19 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>19-06-2024 20:41:45</t>
+          <t>21-06-2024 12:21:40</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Taiwan</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Chinês</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>早上好</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>21-06-2024 12:19:40</t>
+          <t>21-06-2024 12:21:46</t>
         </is>
       </c>
     </row>
@@ -1873,17 +1873,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Chinês</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Que dia é hoje</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>早上好</t>
+          <t>What day is today</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>21-06-2024 12:20:34</t>
+          <t>21-06-2024 12:21:57</t>
         </is>
       </c>
     </row>
@@ -1919,41 +1919,41 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Chinês</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Meu pau na sua mao</t>
+          <t>Bom dia, gostaria de falar com o senhor pedro</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>我的公鸡在你的手里</t>
+          <t>Good morning, i would like to talk to mr. pedro</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>21-06-2024 12:20:45</t>
+          <t>23-06-2024 11:25:11</t>
         </is>
       </c>
     </row>
@@ -1965,225 +1965,225 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Chinês</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Fala direito</t>
+          <t>Seria possível?</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>言语正确</t>
+          <t>It would be possible?</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>21-06-2024 12:20:59</t>
+          <t>23-06-2024 11:25:32</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Taiwan</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Que dia é hoje malandro?</t>
+          <t>Yes, one momento please!</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>今天是哪一天的騙子？</t>
+          <t>Sim, um momento, por favor!</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>21-06-2024 12:21:13</t>
+          <t>23-06-2024 11:25:47</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Taiwan</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Posso me sentar aqui?</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>May i sit here?</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>21-06-2024 12:21:40</t>
+          <t>23-06-2024 11:26:01</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Taiwan</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Yes, feel free</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Bom dia</t>
+          <t>Sim, sinta -se livre</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>21-06-2024 12:21:46</t>
+          <t>23-06-2024 11:26:26</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Que dia é hoje</t>
+          <t>Mr. pedro will talk to you soon, okay?</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>What day is today</t>
+          <t>O sr. pedro falará com você em breve, ok?</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" t="b">
         <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>21-06-2024 12:21:57</t>
+          <t>23-06-2024 11:27:04</t>
         </is>
       </c>
     </row>
@@ -2195,41 +2195,41 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Espanhol</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Fala comigo jão se não eu vou pegar você pelo cangote</t>
+          <t>Que dia é hoje</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Talk to me jão if not i will take you for the neck</t>
+          <t>Qué día es hoy</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Chrome Mobile</t>
+          <t>Chrome</t>
         </is>
       </c>
       <c r="F39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Windows</t>
         </is>
       </c>
       <c r="H39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>21-06-2024 12:22:10</t>
+          <t>23-06-2024 12:17:54</t>
         </is>
       </c>
     </row>
@@ -2241,17 +2241,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Espanhol</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Bom dia, gostaria de falar com o senhor pedro</t>
+          <t>Bom dia</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Good morning, i would like to talk to mr. pedro</t>
+          <t>Buen día</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>23-06-2024 11:25:11</t>
+          <t>23-06-2024 12:17:57</t>
         </is>
       </c>
     </row>
@@ -2287,17 +2287,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Espanhol</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Seria possível?</t>
+          <t>Boa tarde</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>It would be possible?</t>
+          <t>Buenas tardes</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2321,29 +2321,29 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>23-06-2024 11:25:32</t>
+          <t>23-06-2024 12:17:59</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Espanhol</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Yes, one momento please!</t>
+          <t>Amigo</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Sim, um momento, por favor!</t>
+          <t>Amigo</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>23-06-2024 11:25:47</t>
+          <t>23-06-2024 12:18:00</t>
         </is>
       </c>
     </row>
@@ -2379,17 +2379,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Espanhol</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Posso me sentar aqui?</t>
+          <t>Queijo</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>May i sit here?</t>
+          <t>Queso</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2413,29 +2413,29 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>23-06-2024 11:26:01</t>
+          <t>23-06-2024 12:18:03</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Espanhol</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Yes, feel free</t>
+          <t>Amizade</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Sim, sinta -se livre</t>
+          <t>Amistad</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2459,29 +2459,29 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>23-06-2024 11:26:26</t>
+          <t>23-06-2024 12:18:05</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Espanhol</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mr. pedro will talk to you soon, okay?</t>
+          <t>Frango</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>O sr. pedro falará com você em breve, ok?</t>
+          <t>Pollo</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2505,7 +2505,1985 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>23-06-2024 11:27:04</t>
+          <t>23-06-2024 12:18:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Espanhol</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Bitoneira</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Concreto</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Espanhol</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Café</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Café</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Espanhol</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Celular</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Teléfono móvil</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Guerra</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Война</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Comida</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Еда</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Suprimentos</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Запасы</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Дружба</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Feijão</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Фасоль</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Arroz</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Рис</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Carne</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Мясо</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Frango</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Курица</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Bitoneira</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Конкретный</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H57" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Maçã</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Мусор</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H58" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:18:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Picanha</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Стейк с разрывами</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Russo</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Pastel</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Жареная тесто</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H60" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H65" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H66" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H67" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H68" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H69" t="b">
+        <v>1</v>
+      </c>
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H70" t="b">
+        <v>1</v>
+      </c>
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H71" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H72" t="b">
+        <v>1</v>
+      </c>
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Amizade amizade</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>우정 우정</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H73" t="b">
+        <v>1</v>
+      </c>
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Amizade amizade</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>우정 우정</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H74" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" t="b">
+        <v>0</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H75" t="b">
+        <v>1</v>
+      </c>
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Amizade</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>우정</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H76" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" t="b">
+        <v>0</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:19:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>좋은 아침이에요</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H77" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:27:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>좋은 아침입니다. 무엇을 도와드릴까요?</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Bom dia.como posso ajudá-lo?</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H78" t="b">
+        <v>1</v>
+      </c>
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:27:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>제 이름은 크리스토퍼입니다. 채식 음식이 있는지 알고 싶습니다.</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Meu nome é christopher.eu quero saber se há comida vegetariana.</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H79" t="b">
+        <v>1</v>
+      </c>
+      <c r="I79" t="b">
+        <v>0</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:29:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>네, 그렇습니다. 무엇을 주문하시겠어요?</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>É sim.o que você pediria?</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H80" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" t="b">
+        <v>0</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:30:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Bom dia!</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>좋은 아침이에요!</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:31:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>좋은 아침입니다. 무엇을 도와드릴까요?</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Bom dia.como posso ajudá-lo?</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F82" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H82" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" t="b">
+        <v>0</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:31:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Vocês tem comida vegetariana?</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>채식 음식이 있습니까?</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H83" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" t="b">
+        <v>0</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:32:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>주문하고 싶은 것이 있나요?</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Você quer pedir?</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:32:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Vocês tem comida vegetariana?</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>채식 음식이 있습니까?</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H85" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" t="b">
+        <v>0</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:33:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>주문하고 싶은 것이 있나요?</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Você quer pedir?</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H86" t="b">
+        <v>1</v>
+      </c>
+      <c r="I86" t="b">
+        <v>0</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:33:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Vou querer uma salada de alface com azeitonas por favor</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>올리브와 함께 양상추 샐러드를 원할 것입니다</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H87" t="b">
+        <v>1</v>
+      </c>
+      <c r="I87" t="b">
+        <v>0</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:33:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Coreano</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>알겠습니다. 기록되어 있습니다. 실례합니다!</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Tudo bem.está gravado.com licença!</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H88" t="b">
+        <v>1</v>
+      </c>
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>23-06-2024 12:34:33</t>
         </is>
       </c>
     </row>

</xml_diff>